<commit_message>
0324 jpg to webp
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/nyumData.xlsx
+++ b/src/main/resources/Data/nyumData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jangg\IdeaProjects\nyum-tolic\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29318DF7-6DDA-45AF-B116-871F596056FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4067A66-C831-4DB5-92DE-9B943B217894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="533">
   <si>
     <t>분위기 좋은 에스프레소 바</t>
   </si>
@@ -317,9 +317,6 @@
     <t>술,중식</t>
   </si>
   <si>
-    <t>한식,분식</t>
-  </si>
-  <si>
     <t>한식,닭</t>
   </si>
   <si>
@@ -584,9 +581,6 @@
     <t>남경</t>
   </si>
   <si>
-    <t>안주</t>
-  </si>
-  <si>
     <t>지지고</t>
   </si>
   <si>
@@ -1068,34 +1062,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>미방문</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>학교에 가까운 중국집</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>학교 근처 제육중 불향 가장 강합니다.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">학교의 근처의 돼지갈비찜 맛집 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>닭갈비가 먹고싶다면</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>칼국수 맛집 중에 하나</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>간단하게 먹고싶다면 나쁘지 않다.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>분식,배달</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -1104,30 +1070,14 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>밥을 더 먹을 수 있습니다. 분위기도 좋아요</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>초밥</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>근처의 꽤 괜찮은 초밥집</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>회덮밥도 좋은 선택입니다.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>일식</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>근처의 거의 유일한 라멘집</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>마들렌이 맛있습니다.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -1140,50 +1090,18 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>900원 커피가 가성비가 좋다.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>중식,데이트</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>학교 근처의 중국집 2</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>짬뽕을 먹고싶다면 좋은 선택</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>양식,데이트</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>학교근처 국룰 소개팅 장소</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>사각피자 위에 노른자가 올라며 담백하다, tv에도 나온걸로 유명합니다.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>수제버거를 먹고싶다면</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>한상차림이 한상 가득히 나옴</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>무난한 프랜차이즈입니다.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>구운치킨 특성상 조리가 오래걸리기도 합니다.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>부속고기집이며 양이 꽤 괜찮습니다.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -1208,14 +1126,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>학교앞에 있는 치킨가게</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>이디야</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>순대가 수제라 맛있습니다.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -1228,10 +1138,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>가격대비 양이 많음. 조개젓갈 맛있음</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">역 근처 중식집. </t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -1244,10 +1150,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>떡볶이</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>무난한 횟집</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -1256,14 +1158,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>안가봄</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>맘스터치 가끔 늦게 나온다.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>가끔씩 땡김</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -1276,54 +1170,18 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>맛있음. 자리가 없을 수 있다.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>건강해지고 싶다면.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>역 앞에 위치해 학교에서 가긴 멀지만 맛있습니다.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>든든한 해장이 가능</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>롯데리아</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>평범하게 한끼 떼우기 좋아요</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>분식집을 가고싶다면 좋은 선택, tv에도 나왔다. 양 가격 부답없어요</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>여러분이 잘아시는 엽기떡볶이 입니다.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>분위기 좋은데를 고르고 싶다면. 유부초밥이 생각보다 커서 든든해요</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>제육의 불향이 좋아요.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>여러분이 잘아시는 메가커피 입니다.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>빙수를 진짜 추천합니다. 오티로 많이 모이는 집이죠</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>돈이 많은 대학생이라면..돈값은 해요</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -1336,54 +1194,18 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>배고플때 학교에서 찾자.. 기숙사생 최고의 가성비 선택</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>사장님께서 친절하시고 배부르게 한끼 해결 가능해요</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>꼬치가 진짜 맛있고, 술집 분위기도 좋아요. 조용히 한잔하기에 좋아요</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>학교보다 좋은 선택(컴공 이건희가 강력 추천합니다) 퀄리티가 다릅니다</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>가격할인도 짱짱하고 맛있어요</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>집밥먹는 느낌. 국물없는 제육 취향이신분들 여기 괜찮아요</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>호불호 많이 갈리는 부대찌개</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>수타면이 먹을만 해요.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>럭셔리한 분식을 먹고 싶다면?</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>다들 아는 역전그랜드마더맥주</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>성심여대일때 부터 존재하던 피자집. 가격도 괜찮고 먹을만 해요</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>가격 괜찮아서 가는 곳입니다. 가격 대비 맛도 있어요</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>images/남경.webp</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -1721,6 +1543,270 @@
   </si>
   <si>
     <t>images/학교가는길.webp</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>학교에 가장 가까운 중국집. 전 매뉴가 평타이상은 합니다.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>중식,혼밥</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>한식위주로 매뉴가 다양해요. 평범하게 한끼 떼우기 좋아요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>한식,혼밥</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>학교 근처 제육중 불향 가장 강합니다. 돼지 불백도 맛있고 반찬도 맛있는 집. 집밥이 그리울땐..?</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>학교의 근처의 돼지갈비찜 맛집, 내부가 협소하고 시끄럽다는 단점도 있어요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>닭갈비가 먹고싶다면? 점심 특선으로 9000원까지 합니다. 사람들이 잘 모르는 맛집.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>닭 칼국수 맛집 중에 하나. 여름에 판매하는 비빔국수도 일품이에요</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>밥과 비빔 우동이 있다. 가격도 너무 저렴하고 맛이 있어요. 다만 너무 기름져 느끼하실 수도 있어요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>분식,혼밥</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>분식집을 가고싶다면 좋은 선택, tv에도 나왔다. 양 가격 부답없어요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>한식</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>분위기 좋은데를 고르고 싶다면. 유부초밥이 생각보다 커서 든든해요. 개발자 본인 얼굴 만합니다(저 얼굴 커요).</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>밥을 더 먹을 수 있습니다. 분위기도 좋아요. 덮밥 맛집입니다.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>근처의 꽤 괜찮은 초밥집. 가격은 좀 나가지만 학교 상권치고 퀄이 좋은편 입니다.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>제육의 불향이 좋아요. 자극적인 것을 좋아하시면 추천드립니다.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>일식,혼밥</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>가톨릭대 근처에서 회덮밥을 먹고 싶으면 추천.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>근처의 거의 유일한 라멘집. 일본 라면인데 소주가 땡기는 국물.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>900원 커피가 가성비가 좋아요. 가대생들의 카페인을 책임지는 곳.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>비싼 마라전골도 맛있지만, 기본 마라탕이 맛있는곳. 마라탕 혼밥도 가능한 곳.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>학교 근처의 중국집. 남경이 자리가 없으면 여기 갑니다. 남경과 맛은 동일해요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>짬뽕을 먹고싶다면 좋은 선택. 차돌 짬뽕이 진짜 맛있어요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>학교근처 국룰 소개팅 장소. 전 매뉴가 양식이고 대부분 새우가 들어가요. 맛있어요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>정말 맛있는 수제버거를 먹고싶다면? 생각보다 배가 안차서 개발자 본인은 2개 먹습니다.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>양식,혼밥</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>분위기 좋고 가격도 착해요. 마라전골과 유린기가 맛있어요. 다양한 세트가 준비되서 가볼만한 곳,</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>한상차림이 한상 가득히 나옴. 전과 막걸리가 먹고 싶을땐?</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>무난한 프랜차이즈입니다. 개발자 본인이 알바 하면서 느낀.. 안주를 너무 정성스럽게 맛있게 만들어 맥주가 맛있게 느껴지는 곳</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">빙수를 진짜 추천합니다. 오티로 많이 모이는 집이죠. 안주 3+1 이벤트하는 곳 입니다. </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">레트로 감성 가득한 맥주집. 역쪽이라 언제나 사람이 많아요. </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">너무 맛있고 사장님께서도 친절한 집. 분위기가 좋아서 연인이나 소개팅 자리도 가능해요. 1차,2차로도 가능한 곳. </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>생고기 전문점. 가격도 덜 부담스럽고 고기를 구워주셔서 좋아요. 만석이 자주 있는 곳.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>구운치킨 특성상 조리가 오래걸리기도 합니다. 하지만 구은 치킨을 좋아하시는 분들께 추천드립니다.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격 괜찮아서 가는 곳입니다. 가격 대비 맛도 있어요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>직접 구워주시고 가성비도 좋고 고기도 좋아서 단골이 많은 집이에요. 볶음밥은 국룰.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>여러분이 잘 아시는 bbq</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>여러분이 잘 아시는 60계 치킨</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>학교앞에 있는 치킨가게. 전화 포장 주문 시 떡볶이 서비스 나갑니다. 개발자 본인은 치킨 따로먹고 떡볶이는 다음날 먹습니다. 2끼 해결가능!</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>여러분이 잘 아시는 이디야</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>배고플때 학교에서 찾자.. 기숙사생 최고의 가성비 선택. 포장해서 기숙다식당에서 드셔도 좋아요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>한식,분식,혼밥</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격대비 양이 많음. 조개젓갈 맛있음. 사람들이 잘 모르는 칼국수 맛집 중 하나.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>사장님께서 친절하시고 엄청 배부르게 한끼 해결 가능해요. 다만 재료들이 자극적이라 자주 못먹는게 단점입니다.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>여러분이 잘 아시는 신전 떡볶이. 자극적인 떡볶이를 원하시면 추천해요. 긱사 생분들은 1인 메뉴도 추천드릴게요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>역곡의 퀄리티 있는 필터 커피를 즐기고 싶다면..?</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>다들 아는 역전그랜드마더비어</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 안주가 맛있지만 특히 치킨 가라아케가 맛있는 집. 대화하기도 좋은 가게.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>꼬치가 진짜 맛있고, 술집 분위기도 좋아요. 조용히 한잔하기에 좋아요. 저녁에는 자주 매진이 되는 집.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>여기 닭꼬치가 맛있어요. 서비스도 잘 주시는 가게.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>튀김 옷도 얇고 맛있는 집. 하지만 그때그때 맛의 편차가 좀 있다.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 반찬도 맛있고 족발도 야들야들 하니 맛있다. 막국수도 양도 많고 존맛. 술도둑 입니다.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>괜찮다는 평이 많다.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>양식,배달,혼밥</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>학교맘터보다 좋은 선택(컴공 이건희가 매우매우 강력하게 추천합니다) 퀄리티가 다릅니다</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격할인도 짱짱하고 맛있어요. 괜히 장사 잘 되는게 아님</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>학교 국제관 1충에 있는 곳. 여러분이 아시는 메머드 커피.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>수타면이 먹을만 해요. 사장님께서 너무 친절하심!</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>맛있음. 자리가 없을 수 있다. 특히 불향 나는 떡볶이가 일품이에요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>매장이 깔끔하고 조용해서 대화 나누거나 과제하기 좋은 곳.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>호불호 많이 갈리는 부대찌개. 밥이 무한이라서 배 채우기 걱정없어요.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>학교 앞 탕화쿵부처럼 진한 땅콩소스맛 육수 안 좋아하고 라화쿵부나 홍리마라탕처럼 사골육수맛 좋아하는 사람들한테 추천</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>역 앞에 위치해 학교에서 가긴 멀지만 맛있습니다. 특히 모둠 먹으면 진짜 남길정도의 양</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>여러분이 잘 아시는 롯데리아</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>정말 맛있는 뼈감자탕집. 뼈가 사람 뼈마냥 크고 푸짐합니다. 컴공 아저씨들은 일주일에 한번 씩은 가는집.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>혼밥</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -1849,7 +1935,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1897,6 +1983,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2454,7 +2543,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2462,7 +2551,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -2470,7 +2559,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2478,7 +2567,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -2486,7 +2575,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -2494,15 +2583,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -2510,7 +2599,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -2518,7 +2607,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -2526,7 +2615,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -2534,7 +2623,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
@@ -2542,7 +2631,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
@@ -2550,7 +2639,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>187</v>
+        <v>237</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
@@ -2558,18 +2647,18 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>236</v>
+      <c r="A14" s="12" t="s">
+        <v>532</v>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2584,8 +2673,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView topLeftCell="A78" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2600,42 +2689,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="H1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>6</v>
@@ -2644,16 +2733,16 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>349</v>
+        <v>467</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>200</v>
+      <c r="H2" s="12" t="s">
+        <v>468</v>
       </c>
       <c r="I2">
         <v>37.486217440038999</v>
@@ -2662,15 +2751,15 @@
         <v>126.80527293775</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>1</v>
@@ -2679,16 +2768,16 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>405</v>
+        <v>469</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
-        <v>206</v>
+      <c r="H3" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="I3">
         <v>37.485605899757097</v>
@@ -2697,15 +2786,15 @@
         <v>126.80460177190599</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>11</v>
@@ -2714,16 +2803,16 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>350</v>
+        <v>471</v>
       </c>
       <c r="G4">
         <v>8</v>
       </c>
-      <c r="H4" t="s">
-        <v>206</v>
+      <c r="H4" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="I4">
         <v>37.484743157313098</v>
@@ -2732,15 +2821,15 @@
         <v>126.808713984352</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>429</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>7</v>
@@ -2749,10 +2838,10 @@
         <v>4.5</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>351</v>
+        <v>472</v>
       </c>
       <c r="G5">
         <v>9</v>
@@ -2767,15 +2856,15 @@
         <v>126.809960322531</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
@@ -2784,16 +2873,16 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>352</v>
+        <v>473</v>
       </c>
       <c r="G6">
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I6">
         <v>37.485043914860903</v>
@@ -2802,15 +2891,15 @@
         <v>126.809439672441</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>10</v>
@@ -2819,16 +2908,16 @@
         <v>4.5</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>353</v>
+        <v>474</v>
       </c>
       <c r="G7">
         <v>3</v>
       </c>
-      <c r="H7" t="s">
-        <v>206</v>
+      <c r="H7" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="I7">
         <v>37.485259103938198</v>
@@ -2837,7 +2926,7 @@
         <v>126.806024495491</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>432</v>
+        <v>387</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
@@ -2845,7 +2934,7 @@
         <v>91</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>2</v>
@@ -2854,16 +2943,16 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G8">
         <v>6</v>
       </c>
-      <c r="H8" t="s">
-        <v>206</v>
+      <c r="H8" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="I8">
         <v>37.4846394516712</v>
@@ -2872,15 +2961,15 @@
         <v>126.807272653455</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>38</v>
@@ -2889,16 +2978,16 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>354</v>
+        <v>475</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
-        <v>211</v>
+      <c r="H9" s="12" t="s">
+        <v>476</v>
       </c>
       <c r="I9">
         <v>37.486252715190901</v>
@@ -2907,15 +2996,15 @@
         <v>126.804809264423</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>434</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>22</v>
@@ -2924,16 +3013,16 @@
         <v>3.5</v>
       </c>
       <c r="E10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>406</v>
+        <v>477</v>
       </c>
       <c r="G10">
         <v>4</v>
       </c>
-      <c r="H10" t="s">
-        <v>206</v>
+      <c r="H10" s="12" t="s">
+        <v>478</v>
       </c>
       <c r="I10">
         <v>37.485497186636003</v>
@@ -2942,15 +3031,15 @@
         <v>126.806982127745</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>511</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>15</v>
@@ -2959,16 +3048,16 @@
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>407</v>
+        <v>374</v>
       </c>
       <c r="G11">
         <v>8</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="I11">
         <v>37.484953499782101</v>
@@ -2977,15 +3066,15 @@
         <v>126.809244861902</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>435</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>52</v>
@@ -2994,16 +3083,16 @@
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>408</v>
+        <v>479</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="I12">
         <v>37.485489281787402</v>
@@ -3012,15 +3101,15 @@
         <v>126.806281129108</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>436</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>19</v>
@@ -3029,16 +3118,16 @@
         <v>3.5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>357</v>
+        <v>480</v>
       </c>
       <c r="G13">
         <v>6</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="I13">
         <v>37.484376124816201</v>
@@ -3047,15 +3136,15 @@
         <v>126.807406182305</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>437</v>
+        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>32</v>
@@ -3064,16 +3153,16 @@
         <v>3.5</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>359</v>
+        <v>481</v>
       </c>
       <c r="G14">
         <v>9</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="I14">
         <v>37.485087045156199</v>
@@ -3082,15 +3171,15 @@
         <v>126.809645910124</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>438</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>35</v>
@@ -3099,16 +3188,16 @@
         <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>409</v>
+        <v>482</v>
       </c>
       <c r="G15">
         <v>3</v>
       </c>
-      <c r="H15" t="s">
-        <v>198</v>
+      <c r="H15" s="12" t="s">
+        <v>483</v>
       </c>
       <c r="I15">
         <v>37.484322028046897</v>
@@ -3117,15 +3206,15 @@
         <v>126.806007131678</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>439</v>
+        <v>394</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>37</v>
@@ -3134,16 +3223,16 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>360</v>
+        <v>484</v>
       </c>
       <c r="G16">
         <v>6</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="I16">
         <v>37.484822724520697</v>
@@ -3152,15 +3241,15 @@
         <v>126.807775328921</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>440</v>
+        <v>395</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>23</v>
@@ -3169,16 +3258,16 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>362</v>
+        <v>485</v>
       </c>
       <c r="G17">
         <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I17">
         <v>37.484953508909399</v>
@@ -3187,15 +3276,15 @@
         <v>126.809250515218</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>441</v>
+        <v>396</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>33</v>
@@ -3204,10 +3293,10 @@
         <v>3.8</v>
       </c>
       <c r="E18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="G18">
         <v>4</v>
@@ -3222,15 +3311,15 @@
         <v>126.807206921003</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>442</v>
+        <v>397</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>69</v>
@@ -3242,13 +3331,13 @@
         <v>93</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="I19">
         <v>37.485793357720603</v>
@@ -3257,15 +3346,15 @@
         <v>126.804903740664</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>34</v>
@@ -3274,16 +3363,16 @@
         <v>4.5</v>
       </c>
       <c r="E20" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>366</v>
+        <v>486</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I20">
         <v>37.485609802936601</v>
@@ -3292,15 +3381,15 @@
         <v>126.80560241137501</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>444</v>
+        <v>399</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>31</v>
@@ -3309,10 +3398,10 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>410</v>
+        <v>375</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -3327,15 +3416,15 @@
         <v>126.804958775329</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>445</v>
+        <v>400</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>67</v>
@@ -3347,13 +3436,13 @@
         <v>3</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>348</v>
+        <v>487</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="I22">
         <v>37.485784678924702</v>
@@ -3362,15 +3451,15 @@
         <v>126.805104458966</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>49</v>
@@ -3379,16 +3468,16 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>368</v>
+        <v>488</v>
       </c>
       <c r="G23">
         <v>3</v>
       </c>
-      <c r="H23" t="s">
-        <v>200</v>
+      <c r="H23" s="12" t="s">
+        <v>468</v>
       </c>
       <c r="I23">
         <v>37.485472117984301</v>
@@ -3397,33 +3486,33 @@
         <v>126.806804110846</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D24">
         <v>3.5</v>
       </c>
       <c r="E24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>369</v>
+        <v>489</v>
       </c>
       <c r="G24">
         <v>7</v>
       </c>
-      <c r="H24" t="s">
-        <v>200</v>
+      <c r="H24" s="12" t="s">
+        <v>468</v>
       </c>
       <c r="I24">
         <v>37.4876187047714</v>
@@ -3432,15 +3521,15 @@
         <v>126.809540549543</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>448</v>
+        <v>403</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>20</v>
@@ -3449,16 +3538,16 @@
         <v>3.5</v>
       </c>
       <c r="E25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>371</v>
+        <v>490</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="I25">
         <v>37.486371424902799</v>
@@ -3467,15 +3556,15 @@
         <v>126.80440190752201</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>36</v>
@@ -3484,16 +3573,16 @@
         <v>3.5</v>
       </c>
       <c r="E26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>373</v>
+        <v>491</v>
       </c>
       <c r="G26">
         <v>2</v>
       </c>
-      <c r="H26" t="s">
-        <v>205</v>
+      <c r="H26" s="12" t="s">
+        <v>492</v>
       </c>
       <c r="I26">
         <v>37.485452852107699</v>
@@ -3502,7 +3591,7 @@
         <v>126.80604378137799</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>450</v>
+        <v>405</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -3510,7 +3599,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>16</v>
@@ -3519,16 +3608,16 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="G27">
         <v>5</v>
       </c>
       <c r="H27" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I27">
         <v>37.4852771880539</v>
@@ -3537,15 +3626,15 @@
         <v>126.807440616127</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>451</v>
+        <v>406</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>12</v>
@@ -3554,10 +3643,10 @@
         <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>348</v>
+        <v>493</v>
       </c>
       <c r="G28">
         <v>10</v>
@@ -3572,15 +3661,15 @@
         <v>126.811050906527</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>13</v>
@@ -3589,16 +3678,16 @@
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>374</v>
+        <v>494</v>
       </c>
       <c r="G29">
         <v>8</v>
       </c>
       <c r="H29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I29">
         <v>37.485463400737999</v>
@@ -3607,15 +3696,15 @@
         <v>126.809760849471</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>453</v>
+        <v>408</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>25</v>
@@ -3624,16 +3713,16 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>375</v>
+        <v>495</v>
       </c>
       <c r="G30">
         <v>9</v>
       </c>
       <c r="H30" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I30">
         <v>37.485134516293101</v>
@@ -3642,15 +3731,15 @@
         <v>126.80975037669999</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>454</v>
+        <v>409</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>17</v>
@@ -3659,16 +3748,16 @@
         <v>4</v>
       </c>
       <c r="E31" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>411</v>
+        <v>496</v>
       </c>
       <c r="G31">
         <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I31">
         <v>37.485578293433598</v>
@@ -3677,15 +3766,15 @@
         <v>126.811173904604</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>455</v>
+        <v>410</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>24</v>
@@ -3694,16 +3783,16 @@
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>348</v>
+        <v>497</v>
       </c>
       <c r="G32">
         <v>10</v>
       </c>
       <c r="H32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I32">
         <v>37.485546523304997</v>
@@ -3712,15 +3801,15 @@
         <v>126.811026996593</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>456</v>
+        <v>411</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>26</v>
@@ -3729,16 +3818,16 @@
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>348</v>
+        <v>498</v>
       </c>
       <c r="G33">
         <v>8</v>
       </c>
       <c r="H33" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I33">
         <v>37.48501471886</v>
@@ -3747,15 +3836,15 @@
         <v>126.809493453358</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>457</v>
+        <v>412</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>29</v>
@@ -3764,16 +3853,16 @@
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>348</v>
+        <v>499</v>
       </c>
       <c r="G34">
         <v>9</v>
       </c>
       <c r="H34" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I34">
         <v>37.485252269681297</v>
@@ -3782,15 +3871,15 @@
         <v>126.810137333348</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>14</v>
@@ -3799,10 +3888,10 @@
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>376</v>
+        <v>500</v>
       </c>
       <c r="G35">
         <v>8</v>
@@ -3817,15 +3906,15 @@
         <v>126.80940504867399</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>459</v>
+        <v>414</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>21</v>
@@ -3837,13 +3926,13 @@
         <v>90</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>426</v>
+        <v>501</v>
       </c>
       <c r="G36">
         <v>8</v>
       </c>
       <c r="H36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I36">
         <v>37.484953504345803</v>
@@ -3852,15 +3941,15 @@
         <v>126.80924768856001</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>460</v>
+        <v>415</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>41</v>
@@ -3869,16 +3958,16 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>348</v>
+        <v>502</v>
       </c>
       <c r="G37">
         <v>7</v>
       </c>
       <c r="H37" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I37">
         <v>37.485105646383197</v>
@@ -3887,15 +3976,15 @@
         <v>126.80861129985701</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>461</v>
+        <v>416</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>30</v>
@@ -3904,16 +3993,16 @@
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>377</v>
+        <v>356</v>
       </c>
       <c r="G38">
         <v>9</v>
       </c>
       <c r="H38" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I38">
         <v>37.485842245137803</v>
@@ -3922,15 +4011,15 @@
         <v>126.810022772203</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>462</v>
+        <v>417</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>18</v>
@@ -3939,16 +4028,16 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>412</v>
+        <v>376</v>
       </c>
       <c r="G39">
         <v>5</v>
       </c>
       <c r="H39" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I39">
         <v>37.484711799258001</v>
@@ -3957,15 +4046,15 @@
         <v>126.80743641390001</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>463</v>
+        <v>418</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>27</v>
@@ -3974,16 +4063,16 @@
         <v>3.5</v>
       </c>
       <c r="E40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>378</v>
+        <v>357</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="I40">
         <v>37.485713367130501</v>
@@ -3992,15 +4081,15 @@
         <v>126.80557104935301</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>464</v>
+        <v>419</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>28</v>
@@ -4009,16 +4098,16 @@
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>414</v>
+        <v>378</v>
       </c>
       <c r="G41">
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I41">
         <v>37.4864311346047</v>
@@ -4027,15 +4116,15 @@
         <v>126.805094299427</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>465</v>
+        <v>420</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>53</v>
@@ -4044,16 +4133,16 @@
         <v>2.5</v>
       </c>
       <c r="E42" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>413</v>
+        <v>377</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
-      <c r="H42" t="s">
-        <v>206</v>
+      <c r="H42" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="I42">
         <v>37.4855968850514</v>
@@ -4062,15 +4151,15 @@
         <v>126.804598968691</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>466</v>
+        <v>421</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>60</v>
@@ -4079,16 +4168,16 @@
         <v>3.5</v>
       </c>
       <c r="E43" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>379</v>
+        <v>358</v>
       </c>
       <c r="G43">
         <v>6</v>
       </c>
       <c r="H43" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I43">
         <v>37.484507658332703</v>
@@ -4097,15 +4186,15 @@
         <v>126.80795138859099</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>467</v>
+        <v>422</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>86</v>
@@ -4114,16 +4203,16 @@
         <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>348</v>
+        <v>503</v>
       </c>
       <c r="G44">
         <v>6</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
       <c r="I44">
         <v>37.484494157064901</v>
@@ -4132,15 +4221,15 @@
         <v>126.807959903106</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>468</v>
+        <v>423</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>63</v>
@@ -4149,16 +4238,16 @@
         <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>348</v>
+        <v>504</v>
       </c>
       <c r="G45">
         <v>6</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
       <c r="I45">
         <v>37.484494157064901</v>
@@ -4167,15 +4256,15 @@
         <v>126.807959903106</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>469</v>
+        <v>424</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>76</v>
@@ -4184,10 +4273,10 @@
         <v>3</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>381</v>
+        <v>360</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -4202,15 +4291,15 @@
         <v>126.804858279291</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>470</v>
+        <v>425</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>43</v>
@@ -4219,10 +4308,10 @@
         <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>383</v>
+        <v>505</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -4237,15 +4326,15 @@
         <v>126.805126194846</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>471</v>
+        <v>426</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>54</v>
@@ -4254,10 +4343,10 @@
         <v>3</v>
       </c>
       <c r="E48" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>384</v>
+        <v>506</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -4272,15 +4361,15 @@
         <v>126.805043088126</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>472</v>
+        <v>427</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>47</v>
@@ -4289,16 +4378,16 @@
         <v>3.5</v>
       </c>
       <c r="E49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
       <c r="G49">
         <v>8</v>
       </c>
-      <c r="H49" t="s">
-        <v>206</v>
+      <c r="H49" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="I49">
         <v>37.487799763159799</v>
@@ -4307,15 +4396,15 @@
         <v>126.81007293726</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>473</v>
+        <v>428</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>80</v>
@@ -4324,16 +4413,16 @@
         <v>3</v>
       </c>
       <c r="E50" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>425</v>
+        <v>381</v>
       </c>
       <c r="G50">
         <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I50">
         <v>37.485764012101299</v>
@@ -4342,15 +4431,15 @@
         <v>126.80486565653</v>
       </c>
       <c r="K50" s="12" t="s">
-        <v>474</v>
+        <v>429</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>58</v>
@@ -4359,16 +4448,16 @@
         <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>386</v>
+        <v>363</v>
       </c>
       <c r="G51">
         <v>1</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>387</v>
+        <v>364</v>
       </c>
       <c r="I51">
         <v>37.485587896057297</v>
@@ -4377,15 +4466,15 @@
         <v>126.804611712222</v>
       </c>
       <c r="K51" s="12" t="s">
-        <v>475</v>
+        <v>430</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>39</v>
@@ -4394,16 +4483,16 @@
         <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>415</v>
+        <v>507</v>
       </c>
       <c r="G52">
         <v>1</v>
       </c>
-      <c r="H52" t="s">
-        <v>98</v>
+      <c r="H52" s="12" t="s">
+        <v>508</v>
       </c>
       <c r="I52">
         <v>37.485741491693297</v>
@@ -4412,15 +4501,15 @@
         <v>126.804868541803</v>
       </c>
       <c r="K52" s="12" t="s">
-        <v>476</v>
+        <v>431</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>62</v>
@@ -4429,16 +4518,16 @@
         <v>3.5</v>
       </c>
       <c r="E53" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>388</v>
+        <v>509</v>
       </c>
       <c r="G53">
         <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I53">
         <v>37.485717869820199</v>
@@ -4447,15 +4536,15 @@
         <v>126.80556962433501</v>
       </c>
       <c r="K53" s="12" t="s">
-        <v>477</v>
+        <v>432</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>57</v>
@@ -4467,7 +4556,7 @@
         <v>94</v>
       </c>
       <c r="F54" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G54">
         <v>3</v>
@@ -4482,15 +4571,15 @@
         <v>126.80623441389299</v>
       </c>
       <c r="K54" s="12" t="s">
-        <v>478</v>
+        <v>433</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>46</v>
@@ -4499,16 +4588,16 @@
         <v>3</v>
       </c>
       <c r="E55" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>416</v>
+        <v>510</v>
       </c>
       <c r="G55">
         <v>1</v>
       </c>
-      <c r="H55" t="s">
-        <v>211</v>
+      <c r="H55" s="12" t="s">
+        <v>476</v>
       </c>
       <c r="I55">
         <v>37.486280815262703</v>
@@ -4517,15 +4606,15 @@
         <v>126.805457923362</v>
       </c>
       <c r="K55" s="12" t="s">
-        <v>479</v>
+        <v>434</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>59</v>
@@ -4534,16 +4623,16 @@
         <v>3</v>
       </c>
       <c r="E56" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="G56">
         <v>9</v>
       </c>
       <c r="H56" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I56">
         <v>37.485229715068598</v>
@@ -4552,15 +4641,15 @@
         <v>126.810119017007</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>480</v>
+        <v>435</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C57" s="11" t="s">
         <v>61</v>
@@ -4569,16 +4658,16 @@
         <v>3.7</v>
       </c>
       <c r="E57" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="G57">
         <v>3</v>
       </c>
       <c r="H57" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I57">
         <v>37.485806101015598</v>
@@ -4587,15 +4676,15 @@
         <v>126.807177788738</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>481</v>
+        <v>436</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>51</v>
@@ -4604,16 +4693,16 @@
         <v>3</v>
       </c>
       <c r="E58" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="G58">
         <v>9</v>
       </c>
       <c r="H58" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I58">
         <v>37.4856445443829</v>
@@ -4622,15 +4711,15 @@
         <v>126.810346929445</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>482</v>
+        <v>437</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>65</v>
@@ -4639,16 +4728,16 @@
         <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>392</v>
+        <v>511</v>
       </c>
       <c r="G59">
         <v>5</v>
       </c>
-      <c r="H59" t="s">
-        <v>211</v>
+      <c r="H59" s="12" t="s">
+        <v>476</v>
       </c>
       <c r="I59">
         <v>37.484632488894697</v>
@@ -4657,15 +4746,15 @@
         <v>126.807146885097</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>483</v>
+        <v>438</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>64</v>
@@ -4674,16 +4763,16 @@
         <v>3</v>
       </c>
       <c r="E60" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>348</v>
+        <v>512</v>
       </c>
       <c r="G60">
         <v>1</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="I60">
         <v>37.485713029704101</v>
@@ -4692,15 +4781,15 @@
         <v>126.805366114637</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>484</v>
+        <v>439</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>68</v>
@@ -4709,7 +4798,7 @@
         <v>3.6</v>
       </c>
       <c r="E61" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F61" t="s">
         <v>0</v>
@@ -4718,7 +4807,7 @@
         <v>6</v>
       </c>
       <c r="H61" s="14" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="I61">
         <v>37.484983408219797</v>
@@ -4727,15 +4816,15 @@
         <v>126.808239904519</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>485</v>
+        <v>440</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>56</v>
@@ -4744,16 +4833,16 @@
         <v>3</v>
       </c>
       <c r="E62" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>393</v>
+        <v>368</v>
       </c>
       <c r="G62">
         <v>9</v>
       </c>
       <c r="H62" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I62">
         <v>37.485630525260497</v>
@@ -4762,15 +4851,15 @@
         <v>126.81003320175201</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>486</v>
+        <v>441</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>55</v>
@@ -4779,16 +4868,16 @@
         <v>3</v>
       </c>
       <c r="E63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>424</v>
+        <v>513</v>
       </c>
       <c r="G63">
         <v>9</v>
       </c>
       <c r="H63" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I63">
         <v>37.485934863757898</v>
@@ -4797,15 +4886,15 @@
         <v>126.81018789999401</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>487</v>
+        <v>442</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>40</v>
@@ -4814,16 +4903,16 @@
         <v>3</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>394</v>
+        <v>369</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>348</v>
+        <v>514</v>
       </c>
       <c r="G64">
         <v>9</v>
       </c>
       <c r="H64" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I64">
         <v>37.485878582837401</v>
@@ -4832,15 +4921,15 @@
         <v>126.810207829315</v>
       </c>
       <c r="K64" s="12" t="s">
-        <v>488</v>
+        <v>443</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>66</v>
@@ -4849,10 +4938,10 @@
         <v>4</v>
       </c>
       <c r="E65" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>417</v>
+        <v>515</v>
       </c>
       <c r="G65">
         <v>11</v>
@@ -4867,15 +4956,15 @@
         <v>126.811227906865</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>489</v>
+        <v>444</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>48</v>
@@ -4884,10 +4973,10 @@
         <v>3</v>
       </c>
       <c r="E66" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>348</v>
+        <v>516</v>
       </c>
       <c r="G66">
         <v>10</v>
@@ -4902,15 +4991,15 @@
         <v>126.810817196481</v>
       </c>
       <c r="K66" s="12" t="s">
-        <v>490</v>
+        <v>445</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>42</v>
@@ -4922,7 +5011,7 @@
         <v>44</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>348</v>
+        <v>517</v>
       </c>
       <c r="G67">
         <v>9</v>
@@ -4937,15 +5026,15 @@
         <v>126.810871460472</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>491</v>
+        <v>446</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>45</v>
@@ -4954,16 +5043,16 @@
         <v>3</v>
       </c>
       <c r="E68" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>348</v>
+        <v>518</v>
       </c>
       <c r="G68">
         <v>10</v>
       </c>
       <c r="H68" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I68">
         <v>37.486465666514498</v>
@@ -4972,15 +5061,15 @@
         <v>126.81109958965401</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>492</v>
+        <v>447</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>50</v>
@@ -4989,16 +5078,16 @@
         <v>3</v>
       </c>
       <c r="E69" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F69" s="14" t="s">
-        <v>396</v>
+        <v>519</v>
       </c>
       <c r="G69">
         <v>1</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>387</v>
+        <v>520</v>
       </c>
       <c r="I69">
         <v>37.485496488895201</v>
@@ -5007,15 +5096,15 @@
         <v>126.80382330388299</v>
       </c>
       <c r="K69" s="12" t="s">
-        <v>493</v>
+        <v>448</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>74</v>
@@ -5024,16 +5113,16 @@
         <v>3.5</v>
       </c>
       <c r="E70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>418</v>
+        <v>521</v>
       </c>
       <c r="G70">
         <v>8</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>387</v>
+        <v>520</v>
       </c>
       <c r="I70">
         <v>37.484991922466399</v>
@@ -5042,15 +5131,15 @@
         <v>126.80932532433</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>493</v>
+        <v>448</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>78</v>
@@ -5059,16 +5148,16 @@
         <v>2.5</v>
       </c>
       <c r="E71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>397</v>
+        <v>370</v>
       </c>
       <c r="G71">
         <v>7</v>
       </c>
       <c r="H71" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I71">
         <v>37.485500345476098</v>
@@ -5077,15 +5166,15 @@
         <v>126.808925468913</v>
       </c>
       <c r="K71" s="12" t="s">
-        <v>494</v>
+        <v>449</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>89</v>
@@ -5094,16 +5183,16 @@
         <v>3</v>
       </c>
       <c r="E72" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>398</v>
+        <v>371</v>
       </c>
       <c r="G72">
         <v>4</v>
       </c>
       <c r="H72" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I72">
         <v>37.4871579145832</v>
@@ -5112,15 +5201,15 @@
         <v>126.807363706692</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>495</v>
+        <v>450</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>82</v>
@@ -5129,16 +5218,16 @@
         <v>3</v>
       </c>
       <c r="E73" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>419</v>
+        <v>522</v>
       </c>
       <c r="G73">
         <v>5</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
       <c r="I73">
         <v>37.486829916063698</v>
@@ -5147,27 +5236,27 @@
         <v>126.807897389395</v>
       </c>
       <c r="K73" s="12" t="s">
-        <v>496</v>
+        <v>451</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D74">
         <v>3</v>
       </c>
       <c r="E74" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>395</v>
+        <v>523</v>
       </c>
       <c r="G74">
         <v>1</v>
@@ -5182,15 +5271,15 @@
         <v>126.80379346472</v>
       </c>
       <c r="K74" s="12" t="s">
-        <v>497</v>
+        <v>452</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>87</v>
@@ -5199,16 +5288,16 @@
         <v>3</v>
       </c>
       <c r="E75" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>422</v>
+        <v>524</v>
       </c>
       <c r="G75">
         <v>2</v>
       </c>
-      <c r="H75" t="s">
-        <v>200</v>
+      <c r="H75" s="12" t="s">
+        <v>468</v>
       </c>
       <c r="I75">
         <v>37.485465777282897</v>
@@ -5217,15 +5306,15 @@
         <v>126.805684758526</v>
       </c>
       <c r="K75" s="12" t="s">
-        <v>498</v>
+        <v>453</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>77</v>
@@ -5234,16 +5323,16 @@
         <v>3</v>
       </c>
       <c r="E76" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>420</v>
+        <v>379</v>
       </c>
       <c r="G76">
         <v>2</v>
       </c>
-      <c r="H76" t="s">
-        <v>206</v>
+      <c r="H76" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="I76">
         <v>37.4852659867394</v>
@@ -5252,15 +5341,15 @@
         <v>126.806100798082</v>
       </c>
       <c r="K76" s="12" t="s">
-        <v>499</v>
+        <v>454</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>88</v>
@@ -5269,16 +5358,16 @@
         <v>4.2</v>
       </c>
       <c r="E77" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="G77">
         <v>2</v>
       </c>
       <c r="H77" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I77">
         <v>37.485471043818599</v>
@@ -5287,15 +5376,15 @@
         <v>126.806148321831</v>
       </c>
       <c r="K77" s="12" t="s">
-        <v>500</v>
+        <v>455</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>71</v>
@@ -5304,10 +5393,10 @@
         <v>3</v>
       </c>
       <c r="E78" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>348</v>
+        <v>526</v>
       </c>
       <c r="G78">
         <v>3</v>
@@ -5322,15 +5411,15 @@
         <v>126.806456179731</v>
       </c>
       <c r="K78" s="12" t="s">
-        <v>501</v>
+        <v>456</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>83</v>
@@ -5339,7 +5428,7 @@
         <v>3</v>
       </c>
       <c r="E79" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F79" t="s">
         <v>9</v>
@@ -5357,15 +5446,15 @@
         <v>126.807313105798</v>
       </c>
       <c r="K79" s="12" t="s">
-        <v>502</v>
+        <v>457</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>79</v>
@@ -5374,16 +5463,16 @@
         <v>3.7</v>
       </c>
       <c r="E80" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>399</v>
+        <v>372</v>
       </c>
       <c r="G80">
         <v>7</v>
       </c>
-      <c r="H80" t="s">
-        <v>198</v>
+      <c r="H80" s="12" t="s">
+        <v>483</v>
       </c>
       <c r="I80">
         <v>37.4851076652795</v>
@@ -5392,15 +5481,15 @@
         <v>126.808467134276</v>
       </c>
       <c r="K80" s="12" t="s">
-        <v>503</v>
+        <v>458</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>72</v>
@@ -5409,16 +5498,16 @@
         <v>3</v>
       </c>
       <c r="E81" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>421</v>
+        <v>527</v>
       </c>
       <c r="G81">
         <v>7</v>
       </c>
       <c r="H81" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I81">
         <v>37.485008389901601</v>
@@ -5427,15 +5516,15 @@
         <v>126.80836562754401</v>
       </c>
       <c r="K81" s="12" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.4">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>81</v>
@@ -5444,16 +5533,16 @@
         <v>3</v>
       </c>
       <c r="E82" t="s">
-        <v>227</v>
-      </c>
-      <c r="F82" s="14" t="s">
-        <v>348</v>
+        <v>225</v>
+      </c>
+      <c r="F82" s="16" t="s">
+        <v>528</v>
       </c>
       <c r="G82">
         <v>7</v>
       </c>
       <c r="H82" s="14" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="I82">
         <v>37.484883283856099</v>
@@ -5462,15 +5551,15 @@
         <v>126.80900477375801</v>
       </c>
       <c r="K82" s="12" t="s">
-        <v>505</v>
+        <v>460</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C83" s="11" t="s">
         <v>84</v>
@@ -5479,16 +5568,16 @@
         <v>3</v>
       </c>
       <c r="E83" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>423</v>
+        <v>380</v>
       </c>
       <c r="G83">
         <v>9</v>
       </c>
       <c r="H83" s="14" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="I83">
         <v>37.485515772291102</v>
@@ -5497,15 +5586,15 @@
         <v>126.810111226302</v>
       </c>
       <c r="K83" s="12" t="s">
-        <v>506</v>
+        <v>461</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>73</v>
@@ -5514,16 +5603,16 @@
         <v>3</v>
       </c>
       <c r="E84" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>401</v>
+        <v>373</v>
       </c>
       <c r="G84">
         <v>9</v>
       </c>
       <c r="H84" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I84">
         <v>37.485506471362903</v>
@@ -5532,15 +5621,15 @@
         <v>126.809930341669</v>
       </c>
       <c r="K84" s="12" t="s">
-        <v>507</v>
+        <v>462</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>75</v>
@@ -5549,16 +5638,16 @@
         <v>3.9</v>
       </c>
       <c r="E85" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>402</v>
+        <v>529</v>
       </c>
       <c r="G85">
         <v>9</v>
       </c>
       <c r="H85" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I85">
         <v>37.485308791274598</v>
@@ -5567,15 +5656,15 @@
         <v>126.81026721772</v>
       </c>
       <c r="K85" s="12" t="s">
-        <v>508</v>
+        <v>463</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C86" s="11" t="s">
         <v>85</v>
@@ -5584,16 +5673,16 @@
         <v>3</v>
       </c>
       <c r="E86" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>404</v>
+        <v>530</v>
       </c>
       <c r="G86">
         <v>10</v>
       </c>
       <c r="H86" s="14" t="s">
-        <v>387</v>
+        <v>364</v>
       </c>
       <c r="I86">
         <v>37.485678606400697</v>
@@ -5602,15 +5691,15 @@
         <v>126.81051785849201</v>
       </c>
       <c r="K86" s="12" t="s">
-        <v>509</v>
+        <v>464</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B87" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>70</v>
@@ -5619,16 +5708,16 @@
         <v>4</v>
       </c>
       <c r="E87" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>403</v>
+        <v>531</v>
       </c>
       <c r="G87">
         <v>7</v>
       </c>
-      <c r="H87" t="s">
-        <v>206</v>
+      <c r="H87" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="I87">
         <v>37.485336015207501</v>
@@ -5637,13 +5726,13 @@
         <v>126.808989487812</v>
       </c>
       <c r="K87" s="12" t="s">
-        <v>510</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{3E7A6B36-672D-4F5F-AC3E-13196A85D070}"/>
   </hyperlinks>
   <pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>

</xml_diff>